<commit_message>
Add modified and new test data files
</commit_message>
<xml_diff>
--- a/Code/test_data/rawData/TestData.xlsx
+++ b/Code/test_data/rawData/TestData.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nilesh\UOM Projects\ThermoBand-EN1190\Code\test data\rawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subodha\Desktop\Desk\edp\ThermoBand-EN1190\Code\test_data\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A11D3C-8D0F-40C5-B801-78D115327460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE5AE94-49AF-48FF-B370-E1F0C6BFE816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D8CB8639-DC79-4A23-9E75-180144638258}"/>
+    <workbookView xWindow="1836" yWindow="1284" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{D8CB8639-DC79-4A23-9E75-180144638258}"/>
   </bookViews>
   <sheets>
     <sheet name="t1" sheetId="3" r:id="rId1"/>
     <sheet name="t2" sheetId="4" r:id="rId2"/>
+    <sheet name="t3" sheetId="5" r:id="rId3"/>
+    <sheet name="t4" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>actual</t>
   </si>
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,13 +424,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C72F0A5-0BB5-4EB8-9AB6-92B6A65E340C}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>36.5</v>
       </c>
@@ -446,7 +446,7 @@
         <v>32.44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>36.5</v>
       </c>
@@ -454,7 +454,7 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>36.5</v>
       </c>
@@ -462,7 +462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>36.6</v>
       </c>
@@ -470,7 +470,7 @@
         <v>32.630000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>36.5</v>
       </c>
@@ -478,7 +478,7 @@
         <v>32.94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>36.5</v>
       </c>
@@ -486,7 +486,7 @@
         <v>33.31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>36.5</v>
       </c>
@@ -494,7 +494,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>36.6</v>
       </c>
@@ -502,7 +502,7 @@
         <v>32.94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>36.1</v>
       </c>
@@ -510,7 +510,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>36.4</v>
       </c>
@@ -518,7 +518,7 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>36.5</v>
       </c>
@@ -526,7 +526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>36.5</v>
       </c>
@@ -534,7 +534,7 @@
         <v>32.880000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>36.1</v>
       </c>
@@ -542,7 +542,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>36.5</v>
       </c>
@@ -563,9 +563,9 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>36.299999999999997</v>
       </c>
@@ -581,7 +581,7 @@
         <v>31.56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>36.5</v>
       </c>
@@ -589,7 +589,7 @@
         <v>31.94</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>36.5</v>
       </c>
@@ -597,7 +597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>36.299999999999997</v>
       </c>
@@ -605,7 +605,7 @@
         <v>32.130000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>36.200000000000003</v>
       </c>
@@ -613,7 +613,7 @@
         <v>31.94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>36.4</v>
       </c>
@@ -621,7 +621,7 @@
         <v>31.88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>36.5</v>
       </c>
@@ -629,7 +629,7 @@
         <v>32.06</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>36.5</v>
       </c>
@@ -637,7 +637,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>36.6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>32.81</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>36.5</v>
       </c>
@@ -653,7 +653,7 @@
         <v>33.06</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>36.5</v>
       </c>
@@ -661,7 +661,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>36.5</v>
       </c>
@@ -669,7 +669,7 @@
         <v>32.380000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>36.4</v>
       </c>
@@ -677,7 +677,7 @@
         <v>32.69</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>36.4</v>
       </c>
@@ -685,7 +685,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>35.799999999999997</v>
       </c>
@@ -693,12 +693,318 @@
         <v>33.06</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>36.1</v>
       </c>
       <c r="B17">
         <v>33.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDA994E-77F5-4B04-9A49-0FDABF20671D}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>36.1</v>
+      </c>
+      <c r="B2">
+        <v>33.880000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B3">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B4">
+        <v>34.31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="B5">
+        <v>34.31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B6">
+        <v>34.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B7">
+        <v>34.130000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B8">
+        <v>34.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>36.4</v>
+      </c>
+      <c r="B9">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="B10">
+        <v>34.630000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>36.1</v>
+      </c>
+      <c r="B11">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B13">
+        <v>34.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B14">
+        <v>34.630000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>36.1</v>
+      </c>
+      <c r="B15">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>36.1</v>
+      </c>
+      <c r="B16">
+        <v>34.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465ACE05-A2FF-43D2-9DA0-104311AC7196}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="B2">
+        <v>34.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="B3">
+        <v>34.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="B4">
+        <v>34.19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>36.1</v>
+      </c>
+      <c r="B5">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>34.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>36.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>